<commit_message>
Support reading from DirectBuffer. Before the changes reusing buffers from pool caused wrong primitives deserialization when buffers were not cleared on return. Clearing them reduces performance by 2x. Allocating exact buffers for UTF8 payload read from native memory will just kill perf and GC. Now it is possible to read from native memory directly.
Plus performance improvements (inlining, reducing duplicate ops that compiler doesn't know are equivalent, betting on hot paths aggressively).
</commit_message>
<xml_diff>
--- a/docs/graph.xlsx
+++ b/docs/graph.xlsx
@@ -1,30 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neuecc\Documents\neuecc\Utf8Json\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MD\Dev\fi.im\sln\Spreads\lib\Utf8Json\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA80CB5-9BB8-41BE-ACB5-E2528ADF44DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="53925" windowHeight="28320"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Serialize" sheetId="2" r:id="rId2"/>
+    <sheet name="Deserialize" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="108">
   <si>
     <t>Method</t>
   </si>
@@ -39,14 +47,6 @@
   </si>
   <si>
     <t>JsonNet</t>
-  </si>
-  <si>
-    <t>Utf8Json</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>MessagePack</t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>Serialize(ns)</t>
@@ -65,30 +65,322 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>MPC(Ctless)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>protobuf-net</t>
-    <phoneticPr fontId="1"/>
+    <t>Spreads</t>
+  </si>
+  <si>
+    <t>BenchmarkDotNet=v0.11.1, OS=Windows 10.0.17134.112 (1803/April2018Update/Redstone4)</t>
+  </si>
+  <si>
+    <t>Intel Core i7-8700 CPU 3.20GHz (Max: 3.19GHz) (Coffee Lake), 1 CPU, 12 logical and 6 physical cores</t>
+  </si>
+  <si>
+    <t>.NET Core SDK=2.1.402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  [Host]   : .NET Core 2.1.4 (CoreCLR 4.6.26814.03, CoreFX 4.6.26814.02), 64bit RyuJIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ShortRun : .NET Core 2.1.4 (CoreCLR 4.6.26814.03, CoreFX 4.6.26814.02), 64bit RyuJIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Job=ShortRun  Jit=RyuJit  Runtime=Core  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toolchain=.NET Core 2.1  IterationCount=3  LaunchCount=1  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">WarmupCount=3  </t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>StdDev</t>
+  </si>
+  <si>
+    <t>Scaled</t>
+  </si>
+  <si>
+    <t>ScaledSD</t>
+  </si>
+  <si>
+    <t>Gen 0</t>
+  </si>
+  <si>
+    <t>Gen 1</t>
+  </si>
+  <si>
+    <t>Allocated</t>
+  </si>
+  <si>
+    <t>Utf8JsonSerializer</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>176 B</t>
+  </si>
+  <si>
+    <t>SpreadsJsonSerializer</t>
+  </si>
+  <si>
+    <t>MessagePackCSharp</t>
+  </si>
+  <si>
+    <t>64 B</t>
+  </si>
+  <si>
+    <t>MessagePackCSharpContractless</t>
+  </si>
+  <si>
+    <t>Protobufnet</t>
+  </si>
+  <si>
+    <t>560 B</t>
+  </si>
+  <si>
+    <t>1464 B</t>
+  </si>
+  <si>
+    <t>5784 B</t>
+  </si>
+  <si>
+    <t>840 B</t>
+  </si>
+  <si>
+    <t>1984 B</t>
+  </si>
+  <si>
+    <t>48 B</t>
+  </si>
+  <si>
+    <t>120 B</t>
+  </si>
+  <si>
+    <t>464 B</t>
+  </si>
+  <si>
+    <t>JilTextReader</t>
+  </si>
+  <si>
+    <t>3488 B</t>
+  </si>
+  <si>
+    <t>3288 B</t>
+  </si>
+  <si>
+    <t>1032 B</t>
+  </si>
+  <si>
+    <t>Utf8Json</t>
+  </si>
+  <si>
+    <t>Mpack</t>
+  </si>
+  <si>
+    <t>Mpack (CTL)</t>
+  </si>
+  <si>
+    <t>56 B</t>
+  </si>
+  <si>
+    <t>377.66 ns</t>
+  </si>
+  <si>
+    <t>40.39 ns</t>
+  </si>
+  <si>
+    <t>2.2820 ns</t>
+  </si>
+  <si>
+    <t>182.41 ns</t>
+  </si>
+  <si>
+    <t>59.22 ns</t>
+  </si>
+  <si>
+    <t>3.3458 ns</t>
+  </si>
+  <si>
+    <t>77.99 ns</t>
+  </si>
+  <si>
+    <t>11.51 ns</t>
+  </si>
+  <si>
+    <t>0.6505 ns</t>
+  </si>
+  <si>
+    <t>162.18 ns</t>
+  </si>
+  <si>
+    <t>13.60 ns</t>
+  </si>
+  <si>
+    <t>0.7682 ns</t>
+  </si>
+  <si>
+    <t>334.45 ns</t>
+  </si>
+  <si>
+    <t>22.45 ns</t>
+  </si>
+  <si>
+    <t>1.2683 ns</t>
+  </si>
+  <si>
+    <t>712.01 ns</t>
+  </si>
+  <si>
+    <t>49.59 ns</t>
+  </si>
+  <si>
+    <t>2.8017 ns</t>
+  </si>
+  <si>
+    <t>1,063.17 ns</t>
+  </si>
+  <si>
+    <t>43.06 ns</t>
+  </si>
+  <si>
+    <t>2.4330 ns</t>
+  </si>
+  <si>
+    <t>2,830.16 ns</t>
+  </si>
+  <si>
+    <t>218.77 ns</t>
+  </si>
+  <si>
+    <t>12.3612 ns</t>
+  </si>
+  <si>
+    <t>1,171.22 ns</t>
+  </si>
+  <si>
+    <t>137.34 ns</t>
+  </si>
+  <si>
+    <t>7.7598 ns</t>
+  </si>
+  <si>
+    <t>250.03 ns</t>
+  </si>
+  <si>
+    <t>19.578 ns</t>
+  </si>
+  <si>
+    <t>1.1062 ns</t>
+  </si>
+  <si>
+    <t>156.40 ns</t>
+  </si>
+  <si>
+    <t>10.736 ns</t>
+  </si>
+  <si>
+    <t>0.6066 ns</t>
+  </si>
+  <si>
+    <t>80.65 ns</t>
+  </si>
+  <si>
+    <t>14.930 ns</t>
+  </si>
+  <si>
+    <t>0.8436 ns</t>
+  </si>
+  <si>
+    <t>143.62 ns</t>
+  </si>
+  <si>
+    <t>7.962 ns</t>
+  </si>
+  <si>
+    <t>0.4499 ns</t>
+  </si>
+  <si>
+    <t>144 B</t>
+  </si>
+  <si>
+    <t>478.21 ns</t>
+  </si>
+  <si>
+    <t>32.458 ns</t>
+  </si>
+  <si>
+    <t>1.8339 ns</t>
+  </si>
+  <si>
+    <t>504.32 ns</t>
+  </si>
+  <si>
+    <t>10.025 ns</t>
+  </si>
+  <si>
+    <t>0.5664 ns</t>
+  </si>
+  <si>
+    <t>691.25 ns</t>
+  </si>
+  <si>
+    <t>72.427 ns</t>
+  </si>
+  <si>
+    <t>4.0923 ns</t>
+  </si>
+  <si>
+    <t>527.21 ns</t>
+  </si>
+  <si>
+    <t>26.516 ns</t>
+  </si>
+  <si>
+    <t>1.4982 ns</t>
+  </si>
+  <si>
+    <t>1,491.23 ns</t>
+  </si>
+  <si>
+    <t>138.066 ns</t>
+  </si>
+  <si>
+    <t>7.8010 ns</t>
+  </si>
+  <si>
+    <t>vs. JsonNet</t>
+  </si>
+  <si>
+    <t>Write</t>
+  </si>
+  <si>
+    <t>Read</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="170" formatCode="#,##0.0"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -96,7 +388,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -124,19 +416,28 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -154,7 +455,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="ja-JP"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -172,7 +473,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr lang="ja-JP" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -205,7 +506,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr lang="ja-JP" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -217,7 +518,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="ja-JP"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -254,31 +555,34 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$M$17:$M$24</c:f>
+              <c:f>Sheet1!$M$17:$M$25</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>MessagePack</c:v>
+                  <c:v>Mpack</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>MPC(Ctless)</c:v>
+                  <c:v>Mpack (CTL)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>protobuf-net</c:v>
+                  <c:v>Spreads</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>Protobufnet</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>Utf8Json</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Jil</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>JilTextWriter</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>NetJson</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>JsonNet</c:v>
                 </c:pt>
               </c:strCache>
@@ -286,33 +590,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$17:$N$24</c:f>
+              <c:f>Sheet1!$N$17:$N$25</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>127.3</c:v>
+                  <c:v>80.650000000000006</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>140.1</c:v>
+                  <c:v>143.62</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>350</c:v>
+                  <c:v>156.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>305.89999999999998</c:v>
+                  <c:v>478.21</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>774.5</c:v>
+                  <c:v>250.03</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>960.6</c:v>
+                  <c:v>504.32</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>847.2</c:v>
+                  <c:v>691.25</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2163.4</c:v>
+                  <c:v>527.21</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1491.23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -349,31 +656,34 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$M$17:$M$24</c:f>
+              <c:f>Sheet1!$M$17:$M$25</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>MessagePack</c:v>
+                  <c:v>Mpack</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>MPC(Ctless)</c:v>
+                  <c:v>Mpack (CTL)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>protobuf-net</c:v>
+                  <c:v>Spreads</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>Protobufnet</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>Utf8Json</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Jil</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>JilTextWriter</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>NetJson</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>JsonNet</c:v>
                 </c:pt>
               </c:strCache>
@@ -381,33 +691,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$17:$P$24</c:f>
+              <c:f>Sheet1!$P$17:$P$25</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>113</c:v>
+                  <c:v>77.989999999999995</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>191.8</c:v>
+                  <c:v>162.18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>259.39999999999998</c:v>
+                  <c:v>182.41</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>591.79999999999995</c:v>
+                  <c:v>334.45</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>789.3</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="#,##0.00">
-                  <c:v>1403.4</c:v>
+                  <c:v>377.66</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>712.01</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1112.3</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="#,##0.00">
-                  <c:v>3137.7</c:v>
+                  <c:v>1063.17</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1171.22</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2830.16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -461,31 +774,34 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$M$17:$M$24</c:f>
+              <c:f>Sheet1!$M$17:$M$25</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>MessagePack</c:v>
+                  <c:v>Mpack</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>MPC(Ctless)</c:v>
+                  <c:v>Mpack (CTL)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>protobuf-net</c:v>
+                  <c:v>Spreads</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>Protobufnet</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>Utf8Json</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Jil</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>JilTextWriter</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>NetJson</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>JsonNet</c:v>
                 </c:pt>
               </c:strCache>
@@ -493,33 +809,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$17:$O$24</c:f>
+              <c:f>Sheet1!$O$17:$O$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>128</c:v>
+                  <c:v>144</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>536</c:v>
+                  <c:v>176</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>560</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>176</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>1464</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>5890</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>960</c:v>
+                  <c:v>5784</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2016</c:v>
+                  <c:v>840</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1984</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -559,31 +878,34 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$M$17:$M$24</c:f>
+              <c:f>Sheet1!$M$17:$M$25</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>MessagePack</c:v>
+                  <c:v>Mpack</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>MPC(Ctless)</c:v>
+                  <c:v>Mpack (CTL)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>protobuf-net</c:v>
+                  <c:v>Spreads</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>Protobufnet</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>Utf8Json</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Jil</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>JilTextWriter</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>NetJson</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>JsonNet</c:v>
                 </c:pt>
               </c:strCache>
@@ -591,33 +913,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$17:$Q$24</c:f>
+              <c:f>Sheet1!$Q$17:$Q$25</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>48</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>152</c:v>
-                </c:pt>
                 <c:pt idx="3">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>48</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>464</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>3544</c:v>
-                </c:pt>
                 <c:pt idx="6">
+                  <c:v>3488</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>1032</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>3296</c:v>
+                <c:pt idx="8">
+                  <c:v>3288</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -671,7 +996,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="ja-JP" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -683,7 +1008,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ja-JP"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="785181520"/>
@@ -714,7 +1039,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -730,7 +1055,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="ja-JP" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -742,7 +1067,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ja-JP"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="785182504"/>
@@ -772,7 +1097,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="ja-JP" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -784,7 +1109,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ja-JP"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="848339872"/>
@@ -803,6 +1128,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="848343152"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -831,7 +1157,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr rtl="0">
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="ja-JP" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -843,7 +1169,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ja-JP"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
       </c:dTable>
@@ -870,7 +1196,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr lang="ja-JP" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -882,7 +1208,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="ja-JP"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -912,7 +1238,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="ja-JP"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1473,110 +1799,182 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>188015</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>185944</xdr:rowOff>
+      <xdr:colOff>588065</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>33544</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>203338</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>41413</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="グラフ 3">
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="3" name="Group 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC38023B-366C-4A63-AFB8-55C7E1CEF27E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8E19F41-7A69-4C22-A9D2-1D1B95E94370}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>819150</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>200024</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>1524000</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="正方形/長方形 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3E92A66-56C1-4CFC-9004-A9E7C3296846}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="11687175" y="9248774"/>
-          <a:ext cx="704850" cy="1819275"/>
+          <a:off x="7427015" y="5177044"/>
+          <a:ext cx="7298635" cy="4198869"/>
+          <a:chOff x="7026965" y="5138944"/>
+          <a:chExt cx="7298635" cy="4198869"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="38100">
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
+      </xdr:grpSpPr>
+      <xdr:graphicFrame macro="">
+        <xdr:nvGraphicFramePr>
+          <xdr:cNvPr id="4" name="グラフ 3">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC38023B-366C-4A63-AFB8-55C7E1CEF27E}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGraphicFramePr/>
+        </xdr:nvGraphicFramePr>
+        <xdr:xfrm>
+          <a:off x="7026965" y="5138944"/>
+          <a:ext cx="7298635" cy="4198869"/>
+        </xdr:xfrm>
+        <a:graphic>
+          <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+            <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          </a:graphicData>
+        </a:graphic>
+      </xdr:graphicFrame>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="5" name="正方形/長方形 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3E92A66-56C1-4CFC-9004-A9E7C3296846}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9496425" y="6934200"/>
+            <a:ext cx="704850" cy="2085974"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="38100">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="2" name="TextBox 1">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9294DBE-638B-432D-918A-06BAFD408541}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9563100" y="6915150"/>
+            <a:ext cx="722505" cy="609013"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>   OPS</a:t>
+            </a:r>
+            <a:br>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+            </a:br>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>W:</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+              <a:t> +60%</a:t>
+            </a:r>
+            <a:br>
+              <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            </a:br>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+              <a:t>R: +107%</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1871,219 +2269,273 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="L16:AW27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="H16:AW28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T12" sqref="T12"/>
+    <sheetView tabSelected="1" topLeftCell="H22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="7" width="9" style="1"/>
-    <col min="8" max="8" width="30.625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="30.5703125" style="1" customWidth="1"/>
     <col min="9" max="10" width="9" style="1"/>
-    <col min="11" max="11" width="5.875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="5.85546875" style="1" customWidth="1"/>
     <col min="12" max="12" width="9" style="1" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="9" style="1"/>
-    <col min="14" max="14" width="16.125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="24.75" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="16.140625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="24.7109375" style="1" customWidth="1"/>
     <col min="16" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="16" spans="13:17" x14ac:dyDescent="0.4">
+    <row r="16" spans="13:17">
       <c r="M16" t="s">
         <v>0</v>
       </c>
       <c r="N16" t="s">
+        <v>5</v>
+      </c>
+      <c r="O16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P16" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q16" t="s">
         <v>7</v>
       </c>
-      <c r="O16" t="s">
-        <v>8</v>
-      </c>
-      <c r="P16" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q16" t="s">
+    </row>
+    <row r="17" spans="8:49">
+      <c r="H17"/>
+      <c r="M17" t="s">
+        <v>47</v>
+      </c>
+      <c r="N17" s="2">
+        <f>VLOOKUP(M17, Serialize!$K$13:$M$21, 2, 0)</f>
+        <v>80.650000000000006</v>
+      </c>
+      <c r="O17">
+        <f>VLOOKUP(M17, Serialize!$K$13:$M$21, 3, 0)</f>
+        <v>64</v>
+      </c>
+      <c r="P17" s="2">
+        <f>VLOOKUP(M17, Deserialize!$K$13:$M$21, 2, 0)</f>
+        <v>77.989999999999995</v>
+      </c>
+      <c r="Q17" s="2">
+        <f>VLOOKUP(M17, Deserialize!$K$13:$M$21, 3, 0)</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="8:49">
+      <c r="H18"/>
+      <c r="M18" t="s">
+        <v>48</v>
+      </c>
+      <c r="N18" s="2">
+        <f>VLOOKUP(M18, Serialize!$K$13:$M$21, 2, 0)</f>
+        <v>143.62</v>
+      </c>
+      <c r="O18">
+        <f>VLOOKUP(M18, Serialize!$K$13:$M$21, 3, 0)</f>
+        <v>144</v>
+      </c>
+      <c r="P18" s="2">
+        <f>VLOOKUP(M18, Deserialize!$K$13:$M$21, 2, 0)</f>
+        <v>162.18</v>
+      </c>
+      <c r="Q18" s="2">
+        <f>VLOOKUP(M18, Deserialize!$K$13:$M$21, 3, 0)</f>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="8:49">
+      <c r="H19"/>
+      <c r="M19" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="13:49" x14ac:dyDescent="0.4">
-      <c r="M17" t="s">
-        <v>6</v>
-      </c>
-      <c r="N17">
-        <v>127.3</v>
-      </c>
-      <c r="O17">
-        <v>64</v>
-      </c>
-      <c r="P17">
-        <v>113</v>
-      </c>
-      <c r="Q17">
+      <c r="N19" s="2">
+        <f>VLOOKUP(M19, Serialize!$K$13:$M$21, 2, 0)</f>
+        <v>156.4</v>
+      </c>
+      <c r="O19">
+        <f>VLOOKUP(M19, Serialize!$K$13:$M$21, 3, 0)</f>
+        <v>176</v>
+      </c>
+      <c r="P19" s="2">
+        <f>VLOOKUP(M19, Deserialize!$K$13:$M$21, 2, 0)</f>
+        <v>182.41</v>
+      </c>
+      <c r="Q19" s="2">
+        <f>VLOOKUP(M19, Deserialize!$K$13:$M$21, 3, 0)</f>
         <v>48</v>
       </c>
-    </row>
-    <row r="18" spans="13:49" x14ac:dyDescent="0.4">
-      <c r="M18" t="s">
-        <v>11</v>
-      </c>
-      <c r="N18">
-        <v>140.1</v>
-      </c>
-      <c r="O18">
-        <v>128</v>
-      </c>
-      <c r="P18">
-        <v>191.8</v>
-      </c>
-      <c r="Q18">
+      <c r="S19" s="3">
+        <f>N19/N21</f>
+        <v>0.62552493700755907</v>
+      </c>
+      <c r="T19" s="3">
+        <f>P19/P21</f>
+        <v>0.48300058253455486</v>
+      </c>
+    </row>
+    <row r="20" spans="8:49">
+      <c r="H20"/>
+      <c r="M20" t="s">
+        <v>33</v>
+      </c>
+      <c r="N20" s="2">
+        <f>VLOOKUP(M20, Serialize!$K$13:$M$21, 2, 0)</f>
+        <v>478.21</v>
+      </c>
+      <c r="O20">
+        <f>VLOOKUP(M20, Serialize!$K$13:$M$21, 3, 0)</f>
+        <v>560</v>
+      </c>
+      <c r="P20" s="2">
+        <f>VLOOKUP(M20, Deserialize!$K$13:$M$21, 2, 0)</f>
+        <v>334.45</v>
+      </c>
+      <c r="Q20" s="2">
+        <f>VLOOKUP(M20, Deserialize!$K$13:$M$21, 3, 0)</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="8:49">
+      <c r="H21"/>
+      <c r="M21" t="s">
+        <v>46</v>
+      </c>
+      <c r="N21" s="2">
+        <f>VLOOKUP(M21, Serialize!$K$13:$M$21, 2, 0)</f>
+        <v>250.03</v>
+      </c>
+      <c r="O21">
+        <f>VLOOKUP(M21, Serialize!$K$13:$M$21, 3, 0)</f>
+        <v>176</v>
+      </c>
+      <c r="P21" s="2">
+        <f>VLOOKUP(M21, Deserialize!$K$13:$M$21, 2, 0)</f>
+        <v>377.66</v>
+      </c>
+      <c r="Q21" s="2">
+        <f>VLOOKUP(M21, Deserialize!$K$13:$M$21, 3, 0)</f>
         <v>48</v>
       </c>
-    </row>
-    <row r="19" spans="13:49" x14ac:dyDescent="0.4">
-      <c r="M19" t="s">
-        <v>12</v>
-      </c>
-      <c r="N19">
-        <v>350</v>
-      </c>
-      <c r="O19">
-        <v>536</v>
-      </c>
-      <c r="P19">
-        <v>259.39999999999998</v>
-      </c>
-      <c r="Q19">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="20" spans="13:49" x14ac:dyDescent="0.4">
-      <c r="M20" t="s">
-        <v>5</v>
-      </c>
-      <c r="N20">
-        <v>305.89999999999998</v>
-      </c>
-      <c r="O20">
-        <v>176</v>
-      </c>
-      <c r="P20">
-        <v>591.79999999999995</v>
-      </c>
-      <c r="Q20">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="13:49" x14ac:dyDescent="0.4">
-      <c r="M21" t="s">
+      <c r="S21" s="3">
+        <f>N21/N19</f>
+        <v>1.5986572890025574</v>
+      </c>
+      <c r="T21" s="3">
+        <f>P21/P19</f>
+        <v>2.070390877693109</v>
+      </c>
+    </row>
+    <row r="22" spans="8:49">
+      <c r="H22"/>
+      <c r="M22" t="s">
         <v>1</v>
       </c>
-      <c r="N21">
-        <v>774.5</v>
-      </c>
-      <c r="O21">
+      <c r="N22" s="2">
+        <f>VLOOKUP(M22, Serialize!$K$13:$M$21, 2, 0)</f>
+        <v>504.32</v>
+      </c>
+      <c r="O22">
+        <f>VLOOKUP(M22, Serialize!$K$13:$M$21, 3, 0)</f>
         <v>1464</v>
       </c>
-      <c r="P21">
-        <v>789.3</v>
-      </c>
-      <c r="Q21">
+      <c r="P22" s="2">
+        <f>VLOOKUP(M22, Deserialize!$K$13:$M$21, 2, 0)</f>
+        <v>712.01</v>
+      </c>
+      <c r="Q22" s="2">
+        <f>VLOOKUP(M22, Deserialize!$K$13:$M$21, 3, 0)</f>
         <v>464</v>
       </c>
     </row>
-    <row r="22" spans="13:49" x14ac:dyDescent="0.4">
-      <c r="M22" t="s">
+    <row r="23" spans="8:49">
+      <c r="H23"/>
+      <c r="M23" t="s">
         <v>2</v>
       </c>
-      <c r="N22">
-        <v>960.6</v>
-      </c>
-      <c r="O22">
-        <v>5890</v>
-      </c>
-      <c r="P22" s="2">
-        <v>1403.4</v>
-      </c>
-      <c r="Q22">
-        <v>3544</v>
-      </c>
-    </row>
-    <row r="23" spans="13:49" x14ac:dyDescent="0.4">
-      <c r="M23" t="s">
+      <c r="N23" s="2">
+        <f>VLOOKUP(M23, Serialize!$K$13:$M$21, 2, 0)</f>
+        <v>691.25</v>
+      </c>
+      <c r="O23">
+        <f>VLOOKUP(M23, Serialize!$K$13:$M$21, 3, 0)</f>
+        <v>5784</v>
+      </c>
+      <c r="P23" s="2">
+        <f>VLOOKUP(M23, Deserialize!$K$13:$M$21, 2, 0)</f>
+        <v>1063.17</v>
+      </c>
+      <c r="Q23" s="2">
+        <f>VLOOKUP(M23, Deserialize!$K$13:$M$21, 3, 0)</f>
+        <v>3488</v>
+      </c>
+    </row>
+    <row r="24" spans="8:49">
+      <c r="H24" t="s">
+        <v>105</v>
+      </c>
+      <c r="M24" t="s">
         <v>3</v>
       </c>
-      <c r="N23">
-        <v>847.2</v>
-      </c>
-      <c r="O23">
-        <v>960</v>
-      </c>
-      <c r="P23">
-        <v>1112.3</v>
-      </c>
-      <c r="Q23">
+      <c r="N24" s="2">
+        <f>VLOOKUP(M24, Serialize!$K$13:$M$21, 2, 0)</f>
+        <v>527.21</v>
+      </c>
+      <c r="O24">
+        <f>VLOOKUP(M24, Serialize!$K$13:$M$21, 3, 0)</f>
+        <v>840</v>
+      </c>
+      <c r="P24" s="2">
+        <f>VLOOKUP(M24, Deserialize!$K$13:$M$21, 2, 0)</f>
+        <v>1171.22</v>
+      </c>
+      <c r="Q24" s="2">
+        <f>VLOOKUP(M24, Deserialize!$K$13:$M$21, 3, 0)</f>
         <v>1032</v>
       </c>
     </row>
-    <row r="24" spans="13:49" x14ac:dyDescent="0.4">
-      <c r="M24" t="s">
+    <row r="25" spans="8:49">
+      <c r="H25" t="s">
+        <v>106</v>
+      </c>
+      <c r="I25" s="4">
+        <f>N25/N19</f>
+        <v>9.5347186700767264</v>
+      </c>
+      <c r="M25" t="s">
         <v>4</v>
       </c>
-      <c r="N24">
-        <v>2163.4</v>
-      </c>
-      <c r="O24">
-        <v>2016</v>
-      </c>
-      <c r="P24" s="2">
-        <v>3137.7</v>
-      </c>
-      <c r="Q24">
-        <v>3296</v>
-      </c>
-    </row>
-    <row r="25" spans="13:49" x14ac:dyDescent="0.4">
-      <c r="R25"/>
-      <c r="S25"/>
-      <c r="T25"/>
-      <c r="U25"/>
-      <c r="V25"/>
-      <c r="W25"/>
-      <c r="X25"/>
-      <c r="Y25"/>
-      <c r="Z25"/>
-      <c r="AA25"/>
-      <c r="AB25"/>
-      <c r="AC25"/>
-      <c r="AD25"/>
-      <c r="AE25"/>
-      <c r="AF25"/>
-      <c r="AG25"/>
-      <c r="AH25"/>
-      <c r="AI25"/>
-      <c r="AJ25"/>
-      <c r="AK25"/>
-      <c r="AL25"/>
-      <c r="AM25"/>
-      <c r="AN25"/>
-      <c r="AO25"/>
-      <c r="AP25"/>
-      <c r="AQ25"/>
-      <c r="AR25"/>
-      <c r="AS25"/>
-      <c r="AT25"/>
-      <c r="AU25"/>
-      <c r="AV25"/>
-      <c r="AW25"/>
-    </row>
-    <row r="26" spans="13:49" x14ac:dyDescent="0.4">
-      <c r="M26"/>
-      <c r="N26"/>
-      <c r="O26"/>
-      <c r="P26"/>
-      <c r="Q26"/>
+      <c r="N25" s="2">
+        <f>VLOOKUP(M25, Serialize!$K$13:$M$21, 2, 0)</f>
+        <v>1491.23</v>
+      </c>
+      <c r="O25">
+        <f>VLOOKUP(M25, Serialize!$K$13:$M$21, 3, 0)</f>
+        <v>1984</v>
+      </c>
+      <c r="P25" s="2">
+        <f>VLOOKUP(M25, Deserialize!$K$13:$M$21, 2, 0)</f>
+        <v>2830.16</v>
+      </c>
+      <c r="Q25" s="2">
+        <f>VLOOKUP(M25, Deserialize!$K$13:$M$21, 3, 0)</f>
+        <v>3288</v>
+      </c>
+    </row>
+    <row r="26" spans="8:49">
+      <c r="H26" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="I26" s="4">
+        <f>P25/P19</f>
+        <v>15.515377446411929</v>
+      </c>
       <c r="R26"/>
       <c r="S26"/>
       <c r="T26"/>
@@ -2117,7 +2569,7 @@
       <c r="AV26"/>
       <c r="AW26"/>
     </row>
-    <row r="27" spans="13:49" x14ac:dyDescent="0.4">
+    <row r="27" spans="8:49">
       <c r="M27"/>
       <c r="N27"/>
       <c r="O27"/>
@@ -2152,6 +2604,45 @@
       <c r="AR27"/>
       <c r="AS27"/>
       <c r="AT27"/>
+      <c r="AU27"/>
+      <c r="AV27"/>
+      <c r="AW27"/>
+    </row>
+    <row r="28" spans="8:49">
+      <c r="M28"/>
+      <c r="N28"/>
+      <c r="O28"/>
+      <c r="P28"/>
+      <c r="Q28"/>
+      <c r="R28"/>
+      <c r="S28"/>
+      <c r="T28"/>
+      <c r="U28"/>
+      <c r="V28"/>
+      <c r="W28"/>
+      <c r="X28"/>
+      <c r="Y28"/>
+      <c r="Z28"/>
+      <c r="AA28"/>
+      <c r="AB28"/>
+      <c r="AC28"/>
+      <c r="AD28"/>
+      <c r="AE28"/>
+      <c r="AF28"/>
+      <c r="AG28"/>
+      <c r="AH28"/>
+      <c r="AI28"/>
+      <c r="AJ28"/>
+      <c r="AK28"/>
+      <c r="AL28"/>
+      <c r="AM28"/>
+      <c r="AN28"/>
+      <c r="AO28"/>
+      <c r="AP28"/>
+      <c r="AQ28"/>
+      <c r="AR28"/>
+      <c r="AS28"/>
+      <c r="AT28"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -2159,4 +2650,898 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECB00DB9-4298-4B71-B221-98B8E3DF1FE8}">
+  <dimension ref="A2:M21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="89.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>2.7699999999999999E-2</v>
+      </c>
+      <c r="H13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I13" t="s">
+        <v>28</v>
+      </c>
+      <c r="K13" t="s">
+        <v>46</v>
+      </c>
+      <c r="L13">
+        <f>LEFT(B13, LEN(B13) - 3)*1</f>
+        <v>250.03</v>
+      </c>
+      <c r="M13">
+        <f>LEFT(I13, LEN(I13) - 2)*1</f>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" t="s">
+        <v>82</v>
+      </c>
+      <c r="E14">
+        <v>0.63</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>2.7900000000000001E-2</v>
+      </c>
+      <c r="H14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K14" t="s">
+        <v>9</v>
+      </c>
+      <c r="L14">
+        <f t="shared" ref="L14:L21" si="0">LEFT(B14, LEN(B14) - 3)*1</f>
+        <v>156.4</v>
+      </c>
+      <c r="M14">
+        <f t="shared" ref="M14:M21" si="1">LEFT(I14, LEN(I14) - 2)*1</f>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15">
+        <v>0.32</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>1.01E-2</v>
+      </c>
+      <c r="H15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" t="s">
+        <v>31</v>
+      </c>
+      <c r="K15" t="s">
+        <v>47</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>80.650000000000006</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>2.2599999999999999E-2</v>
+      </c>
+      <c r="H16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" t="s">
+        <v>89</v>
+      </c>
+      <c r="K16" t="s">
+        <v>48</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>143.62</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="1"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D17" t="s">
+        <v>92</v>
+      </c>
+      <c r="E17">
+        <v>1.91</v>
+      </c>
+      <c r="F17">
+        <v>0.01</v>
+      </c>
+      <c r="G17">
+        <v>8.8700000000000001E-2</v>
+      </c>
+      <c r="H17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I17" t="s">
+        <v>34</v>
+      </c>
+      <c r="K17" t="s">
+        <v>33</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>478.21</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="1"/>
+        <v>560</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>93</v>
+      </c>
+      <c r="C18" t="s">
+        <v>94</v>
+      </c>
+      <c r="D18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E18">
+        <v>2.02</v>
+      </c>
+      <c r="F18">
+        <v>0.01</v>
+      </c>
+      <c r="G18">
+        <v>0.23169999999999999</v>
+      </c>
+      <c r="H18" t="s">
+        <v>27</v>
+      </c>
+      <c r="I18" t="s">
+        <v>35</v>
+      </c>
+      <c r="K18" t="s">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>504.32</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="1"/>
+        <v>1464</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" t="s">
+        <v>98</v>
+      </c>
+      <c r="E19">
+        <v>2.76</v>
+      </c>
+      <c r="F19">
+        <v>0.02</v>
+      </c>
+      <c r="G19">
+        <v>0.91839999999999999</v>
+      </c>
+      <c r="H19">
+        <v>1E-3</v>
+      </c>
+      <c r="I19" t="s">
+        <v>36</v>
+      </c>
+      <c r="K19" t="s">
+        <v>2</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="0"/>
+        <v>691.25</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="1"/>
+        <v>5784</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>99</v>
+      </c>
+      <c r="C20" t="s">
+        <v>100</v>
+      </c>
+      <c r="D20" t="s">
+        <v>101</v>
+      </c>
+      <c r="E20">
+        <v>2.11</v>
+      </c>
+      <c r="F20">
+        <v>0.01</v>
+      </c>
+      <c r="G20">
+        <v>0.1326</v>
+      </c>
+      <c r="H20" t="s">
+        <v>27</v>
+      </c>
+      <c r="I20" t="s">
+        <v>37</v>
+      </c>
+      <c r="K20" t="s">
+        <v>3</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="0"/>
+        <v>527.21</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="1"/>
+        <v>840</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>102</v>
+      </c>
+      <c r="C21" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" t="s">
+        <v>104</v>
+      </c>
+      <c r="E21">
+        <v>5.96</v>
+      </c>
+      <c r="F21">
+        <v>0.03</v>
+      </c>
+      <c r="G21">
+        <v>0.31469999999999998</v>
+      </c>
+      <c r="H21" t="s">
+        <v>27</v>
+      </c>
+      <c r="I21" t="s">
+        <v>38</v>
+      </c>
+      <c r="K21" t="s">
+        <v>4</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="0"/>
+        <v>1491.23</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="1"/>
+        <v>1984</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AF54647-BF11-45D0-8DEC-22F288FC92AE}">
+  <dimension ref="A2:M21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="89.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>7.1999999999999998E-3</v>
+      </c>
+      <c r="H13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I13" t="s">
+        <v>39</v>
+      </c>
+      <c r="K13" t="s">
+        <v>46</v>
+      </c>
+      <c r="L13">
+        <f>LEFT(B13, LEN(B13) - 3)*1</f>
+        <v>377.66</v>
+      </c>
+      <c r="M13">
+        <f>LEFT(I13, LEN(I13) - 2)*1</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14">
+        <v>0.48</v>
+      </c>
+      <c r="F14">
+        <v>0.01</v>
+      </c>
+      <c r="G14">
+        <v>7.4000000000000003E-3</v>
+      </c>
+      <c r="H14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I14" t="s">
+        <v>39</v>
+      </c>
+      <c r="K14" t="s">
+        <v>9</v>
+      </c>
+      <c r="L14">
+        <f t="shared" ref="L14:L21" si="0">LEFT(B14, LEN(B14) - 3)*1</f>
+        <v>182.41</v>
+      </c>
+      <c r="M14">
+        <f t="shared" ref="M14:M21" si="1">LEFT(I14, LEN(I14) - 2)*1</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15">
+        <v>0.21</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="H15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K15" t="s">
+        <v>47</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>77.989999999999995</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16">
+        <v>0.43</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>8.8000000000000005E-3</v>
+      </c>
+      <c r="H16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" t="s">
+        <v>49</v>
+      </c>
+      <c r="K16" t="s">
+        <v>48</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>162.18</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17">
+        <v>0.89</v>
+      </c>
+      <c r="F17">
+        <v>0.01</v>
+      </c>
+      <c r="G17">
+        <v>1.8599999999999998E-2</v>
+      </c>
+      <c r="H17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I17" t="s">
+        <v>40</v>
+      </c>
+      <c r="K17" t="s">
+        <v>33</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>334.45</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18">
+        <v>1.89</v>
+      </c>
+      <c r="F18">
+        <v>0.01</v>
+      </c>
+      <c r="G18">
+        <v>7.3400000000000007E-2</v>
+      </c>
+      <c r="H18" t="s">
+        <v>27</v>
+      </c>
+      <c r="I18" t="s">
+        <v>41</v>
+      </c>
+      <c r="K18" t="s">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>712.01</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="1"/>
+        <v>464</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19">
+        <v>2.82</v>
+      </c>
+      <c r="F19">
+        <v>0.01</v>
+      </c>
+      <c r="G19">
+        <v>0.55310000000000004</v>
+      </c>
+      <c r="H19">
+        <v>1.9E-3</v>
+      </c>
+      <c r="I19" t="s">
+        <v>43</v>
+      </c>
+      <c r="K19" t="s">
+        <v>2</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="0"/>
+        <v>1063.17</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="1"/>
+        <v>3488</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20">
+        <v>7.49</v>
+      </c>
+      <c r="F20">
+        <v>0.05</v>
+      </c>
+      <c r="G20">
+        <v>0.51880000000000004</v>
+      </c>
+      <c r="H20" t="s">
+        <v>27</v>
+      </c>
+      <c r="I20" t="s">
+        <v>44</v>
+      </c>
+      <c r="K20" t="s">
+        <v>4</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="0"/>
+        <v>2830.16</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="1"/>
+        <v>3288</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21">
+        <v>3.1</v>
+      </c>
+      <c r="F21">
+        <v>0.02</v>
+      </c>
+      <c r="G21">
+        <v>0.16209999999999999</v>
+      </c>
+      <c r="H21" t="s">
+        <v>27</v>
+      </c>
+      <c r="I21" t="s">
+        <v>45</v>
+      </c>
+      <c r="K21" t="s">
+        <v>3</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="0"/>
+        <v>1171.22</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="1"/>
+        <v>1032</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>